<commit_message>
Add new column 'Correction ' to Card24 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,7 +521,12 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Event </t>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Correction </t>
         </is>
       </c>
     </row>
@@ -586,7 +591,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -649,7 +659,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -712,7 +727,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -775,7 +795,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -838,7 +863,12 @@
           <t>20\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -901,7 +931,12 @@
           <t>6\10\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -964,7 +999,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1027,7 +1067,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr"/>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1090,7 +1135,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr"/>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1153,7 +1203,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr"/>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1216,7 +1271,12 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr"/>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Edit sheet Card24 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -526,7 +526,7 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Correction </t>
+          <t>Correction</t>
         </is>
       </c>
     </row>
@@ -596,7 +596,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -664,7 +668,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr"/>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -732,7 +740,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr"/>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -800,7 +812,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr"/>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -868,7 +884,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr"/>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -936,7 +956,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr"/>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1004,7 +1028,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr"/>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1072,7 +1100,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr"/>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1140,7 +1172,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr"/>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1208,7 +1244,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr"/>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1276,7 +1316,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr"/>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new row under range 0-150 in Card24 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -610,69 +610,41 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>150</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>99</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>done</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t xml:space="preserve"> تم معايره </t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -682,12 +654,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>301</t>
+          <t>151</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>450</t>
+          <t>300</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -737,7 +709,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>تم تشغيل</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -754,12 +726,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>451</t>
+          <t>301</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>550</t>
+          <t>450</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -809,7 +781,7 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>تم تشغيل</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -826,17 +798,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>551</t>
+          <t>451</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>550</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>632</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -846,22 +818,22 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>✔</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -876,7 +848,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>20\5\2025</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -898,17 +870,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>701</t>
+          <t>551</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>850</t>
+          <t>700</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>870</t>
+          <t>632</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -928,27 +900,27 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>6\10\2025</t>
+          <t>20\5\2025</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -970,57 +942,57 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>851</t>
+          <t>701</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>850</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>870</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>6\10\2025</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -1042,12 +1014,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1001</t>
+          <t>851</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1150</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1114,12 +1086,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1151</t>
+          <t>1001</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1300</t>
+          <t>1150</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1186,12 +1158,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1301</t>
+          <t>1151</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1450</t>
+          <t>1300</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1258,65 +1230,137 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>1451</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="J13" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="K13" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
+      <c r="L13" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr">
+      <c r="M13" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr">
+      <c r="N13" t="inlineStr">
         <is>
           <t>nan</t>
         </is>

</xml_diff>

<commit_message>
Add new column 'event' to Card24 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,6 +529,11 @@
           <t>Correction</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>event</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -591,8 +596,17 @@
           <t>1\1\1111\</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>تم تشغيل ماكينه</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>لايوجد</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -665,6 +679,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -737,6 +752,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -809,6 +825,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -881,6 +898,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -953,6 +971,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1025,6 +1044,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1097,6 +1117,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1169,6 +1190,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1241,6 +1263,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1313,6 +1336,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Serviced by' to Card24 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,6 +529,11 @@
           <t>Correction</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Serviced by</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -601,6 +606,7 @@
           <t>لايوجد</t>
         </is>
       </c>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -673,6 +679,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -745,6 +752,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -817,6 +825,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -889,6 +898,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -961,6 +971,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1033,6 +1044,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1105,6 +1117,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1177,6 +1190,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1249,6 +1263,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1321,22 +1336,7 @@
           <t>nan</t>
         </is>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Serviced by ' to Card24 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,6 +529,11 @@
           <t>Correction</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Serviced by </t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -601,6 +606,7 @@
           <t>لايوجد</t>
         </is>
       </c>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -673,6 +679,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -745,6 +752,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -817,6 +825,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -889,6 +898,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -961,6 +971,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1033,6 +1044,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1105,6 +1117,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1177,6 +1190,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1249,6 +1263,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1321,6 +1336,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'Servised by' to Card24 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,6 +529,11 @@
           <t>Correction</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Servised by</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -601,6 +606,7 @@
           <t>لايوجد</t>
         </is>
       </c>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -673,6 +679,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -745,6 +752,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -817,6 +825,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -886,9 +895,10 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>عطل</t>
-        </is>
-      </c>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -961,6 +971,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1033,6 +1044,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1105,6 +1117,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1177,6 +1190,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1249,6 +1263,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1321,6 +1336,7 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add new column 'event' to Card1 by admin
</commit_message>
<xml_diff>
--- a/Machine_Service_Lookup.xlsx
+++ b/Machine_Service_Lookup.xlsx
@@ -531,67 +531,35 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A2" t="n">
+        <v>24</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>150</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
           <t>1\1\1111\</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>تم تشغيل ماكينه</t>
+        </is>
+      </c>
       <c r="N2" t="inlineStr">
         <is>
           <t>لايوجد</t>
@@ -599,235 +567,89 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A3" t="n">
+        <v>24</v>
+      </c>
+      <c r="B3" t="n">
+        <v>151</v>
+      </c>
+      <c r="C3" t="n">
+        <v>300</v>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>301</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>450</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A4" t="n">
+        <v>24</v>
+      </c>
+      <c r="B4" t="n">
+        <v>301</v>
+      </c>
+      <c r="C4" t="n">
+        <v>450</v>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>تم تشغيل</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>451</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>550</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A5" t="n">
+        <v>24</v>
+      </c>
+      <c r="B5" t="n">
+        <v>451</v>
+      </c>
+      <c r="C5" t="n">
+        <v>550</v>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>551</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>632</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A6" t="n">
+        <v>24</v>
+      </c>
+      <c r="B6" t="n">
+        <v>551</v>
+      </c>
+      <c r="C6" t="n">
+        <v>700</v>
+      </c>
+      <c r="D6" t="n">
+        <v>632</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
           <t>✔</t>
@@ -848,54 +670,30 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>20\5\2025</t>
         </is>
       </c>
       <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>701</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>850</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>870</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A7" t="n">
+        <v>24</v>
+      </c>
+      <c r="B7" t="n">
+        <v>701</v>
+      </c>
+      <c r="C7" t="n">
+        <v>850</v>
+      </c>
+      <c r="D7" t="n">
+        <v>870</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -906,377 +704,127 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
           <t>6\10\2025</t>
         </is>
       </c>
       <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>851</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A8" t="n">
+        <v>24</v>
+      </c>
+      <c r="B8" t="n">
+        <v>851</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>1001</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>1150</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A9" t="n">
+        <v>24</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1001</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1150</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>1151</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>1300</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A10" t="n">
+        <v>24</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1151</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>1301</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1450</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A11" t="n">
+        <v>24</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1301</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1450</v>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>1451</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A12" t="n">
+        <v>24</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1451</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7469,7 +7017,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7538,39 +7086,95 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>event</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>150</v>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>151</v>
-      </c>
-      <c r="C3" t="n">
-        <v>300</v>
-      </c>
-      <c r="D3" t="n">
-        <v>159</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>159</t>
+        </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -7582,48 +7186,122 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>15\7\2024</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" t="n">
-        <v>301</v>
-      </c>
-      <c r="C4" t="n">
-        <v>450</v>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" t="n">
-        <v>451</v>
-      </c>
-      <c r="C5" t="n">
-        <v>550</v>
-      </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -7639,77 +7317,147 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>29\1\2025</t>
         </is>
       </c>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" t="n">
-        <v>551</v>
-      </c>
-      <c r="C6" t="n">
-        <v>700</v>
-      </c>
-      <c r="D6" t="n">
-        <v>565</v>
-      </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>565</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="J6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr"/>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>5\4\2025</t>
         </is>
       </c>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" t="n">
-        <v>701</v>
-      </c>
-      <c r="C7" t="n">
-        <v>850</v>
-      </c>
-      <c r="D7" t="n">
-        <v>724</v>
-      </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>724</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="K7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -7720,116 +7468,322 @@
           <t>5\7\2025</t>
         </is>
       </c>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>1</v>
-      </c>
-      <c r="B8" t="n">
-        <v>851</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D8" t="n">
-        <v>859</v>
-      </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>859</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G8" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L8" t="inlineStr">
         <is>
           <t>24\9\2025</t>
         </is>
       </c>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>1</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1150</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>1</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1151</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>1</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1301</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1450</v>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>1</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1451</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>